<commit_message>
rename `Term` to `Expression` in FormalAmpersand
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Expressions.xlsx
+++ b/AmpersandData/FormalAmpersand/Expressions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Concepts" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="Expressions" sheetId="5" r:id="rId7"/>
     <sheet name="Compositions" sheetId="8" r:id="rId8"/>
     <sheet name="Intersections" sheetId="9" r:id="rId9"/>
+    <sheet name="Contexts" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="45">
   <si>
     <t>[Concept]</t>
   </si>
@@ -151,6 +152,12 @@
   </si>
   <si>
     <t>[Expression]</t>
+  </si>
+  <si>
+    <t>[Context]</t>
+  </si>
+  <si>
+    <t>relations</t>
   </si>
 </sst>
 </file>
@@ -548,12 +555,67 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,7 +798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>